<commit_message>
Databehandling og diskussion af exp2
</commit_message>
<xml_diff>
--- a/Databehandling/Forsøg 2/Sammenhænge.xlsx
+++ b/Databehandling/Forsøg 2/Sammenhænge.xlsx
@@ -26,12 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>$\sqrt{\frac{k}{m}}$</t>
-  </si>
-  <si>
     <t>$\phi$</t>
   </si>
   <si>
@@ -41,9 +35,6 @@
     <t>RMSE</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>Forsøg A</t>
   </si>
   <si>
@@ -57,6 +48,15 @@
   </si>
   <si>
     <t>Forsøg E</t>
+  </si>
+  <si>
+    <t>$b$</t>
+  </si>
+  <si>
+    <t>$A$</t>
+  </si>
+  <si>
+    <t>$a$</t>
   </si>
 </sst>
 </file>
@@ -410,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="244" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="225" workbookViewId="0">
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,27 +423,27 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>-5.858E-2</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>-6.6140000000000004E-2</v>
@@ -489,7 +489,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>-8.0009999999999998E-2</v>
@@ -512,7 +512,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>-6.5060000000000007E-2</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>-6.3579999999999998E-2</v>

</xml_diff>